<commit_message>
A copi of Gender Identity shortlist to translate to norwegian
</commit_message>
<xml_diff>
--- a/data/gender identity/Gender_identity_ShortList_Categorized.xlsx
+++ b/data/gender identity/Gender_identity_ShortList_Categorized.xlsx
@@ -1042,7 +1042,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1058,15 +1058,8 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1124,13 +1117,13 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2092,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="2"/>
       <c r="B16" s="6">
         <v>28</v>
@@ -2134,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="2"/>
       <c r="B17" s="6">
         <v>29</v>
@@ -2176,7 +2169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="2"/>
       <c r="B18" s="6">
         <v>32</v>
@@ -2218,7 +2211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="2"/>
       <c r="B19" s="6">
         <v>33</v>
@@ -2260,7 +2253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="2"/>
       <c r="B20" s="6">
         <v>36</v>
@@ -2302,7 +2295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="2"/>
       <c r="B21" s="6">
         <v>37</v>

</xml_diff>